<commit_message>
added 10 more words but accuracy still needs to be worked on
</commit_message>
<xml_diff>
--- a/translate/record of results.xlsx
+++ b/translate/record of results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\COS301\Hands-Up\translate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5207401C-6B81-49A4-82C0-C41DE59A487A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E52D3B7-7D9E-484F-B13A-C4A11BF87C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,80 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="19">
+  <si>
+    <t>sign</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">predicted </t>
+  </si>
+  <si>
+    <t>accuracy of predicted</t>
+  </si>
+  <si>
+    <t>accuracy of actual sign</t>
+  </si>
+  <si>
+    <t>chair</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cat </t>
+  </si>
+  <si>
+    <t>cold</t>
+  </si>
+  <si>
+    <t>child</t>
+  </si>
+  <si>
+    <t>come</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Test 4</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -66,13 +136,400 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="40">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -83,6 +540,54 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DD2ABC0D-50C1-49C4-8D3A-5CA063F1F218}" name="Table5" displayName="Table5" ref="A2:D12" headerRowCount="0" totalsRowShown="0" dataDxfId="34" tableBorderDxfId="39">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F400AB7F-4E8B-4125-9E25-5ED9FB65B14F}" name="Column1" headerRowDxfId="30" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{3F22CA1A-5693-4313-92A4-EE54C2FDC4CF}" name="Test 1" headerRowDxfId="31" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{788734D9-F3D0-4322-87BC-6A1CAF964241}" name="Column2" headerRowDxfId="32" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{4FC0C234-7164-459C-8403-515A895D477E}" name="Column3" headerRowDxfId="33" dataDxfId="35"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E569A974-8B60-4556-8570-6A44C4FBD727}" name="Table57" displayName="Table57" ref="A16:D26" headerRowCount="0" totalsRowShown="0" dataDxfId="29" tableBorderDxfId="28">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{8766D2EA-8EEA-45A1-8B07-7FA7D5ACC38E}" name="Column1" headerRowDxfId="27" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{A099EBA9-F36A-46FA-BDB1-F7CAF089E494}" name="Test 1" headerRowDxfId="25" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{92A9AE78-3CB8-4AAA-8266-990E00ABEE53}" name="Column2" headerRowDxfId="23" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{8468543C-F567-482E-BE69-7F793167F224}" name="Column3" headerRowDxfId="21" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1C6A1CC9-8976-4B5C-B94C-E8A89F240FFB}" name="Table578" displayName="Table578" ref="A29:D39" headerRowCount="0" totalsRowShown="0" dataDxfId="19" tableBorderDxfId="18">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E504D3A5-FC9A-45F6-8C0E-D7A50AF19A75}" name="Column1" headerRowDxfId="17" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{6EAF6B0D-E32F-4ABE-93B4-E394AE2A7E61}" name="Test 1" headerRowDxfId="15" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{8BDDF0B1-E9A5-48D4-B164-ADE5E3372319}" name="Column2" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{CD0DB33E-E98F-4D80-969C-C6CB71E17312}" name="Column3" headerRowDxfId="11" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{2B773CE3-EB5B-45E6-9DCA-44D0A01FB542}" name="Table5789" displayName="Table5789" ref="A42:D52" headerRowCount="0" totalsRowShown="0" dataDxfId="9" tableBorderDxfId="8">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{DC2E491C-2CD4-4E89-AC71-91DE1A7E1452}" name="Column1" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{BE664661-355B-4988-923D-8558A307F1DC}" name="Test 1" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{E149DA85-C608-4816-AFAC-5502546D39B6}" name="Column2" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{0BD5DA97-7603-4D27-9BC6-3BFD8A154644}" name="Column3" headerRowDxfId="1" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,14 +907,618 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBF13E0-78B5-4465-B2C7-E04C9FCCA561}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.87009999999999998</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.39140000000000003</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.39140000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.73709999999999998</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.3899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.27089999999999997</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4.4900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.25169999999999998</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.1479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.56969999999999998</v>
+      </c>
+      <c r="D10" s="2">
+        <v>8.0399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.37980000000000003</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.37980000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.75019999999999998</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.78E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.99929999999999997</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.48870000000000002</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.1956</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.81379999999999997</v>
+      </c>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.97309999999999997</v>
+      </c>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.95289999999999997</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.91779999999999995</v>
+      </c>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.98150000000000004</v>
+      </c>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.96279999999999999</v>
+      </c>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.51780000000000004</v>
+      </c>
+      <c r="D51" s="2">
+        <v>7.85E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1</v>
+      </c>
+      <c r="D52" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
20 words 40% training accuracy and 8/20 words working
</commit_message>
<xml_diff>
--- a/translate/record of results.xlsx
+++ b/translate/record of results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\COS301\Hands-Up\translate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E52D3B7-7D9E-484F-B13A-C4A11BF87C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE64FEAA-B054-4002-A60D-E39A4FFAA788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
+    <workbookView xWindow="11088" yWindow="552" windowWidth="8688" windowHeight="8880" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="43">
   <si>
     <t>sign</t>
   </si>
@@ -93,6 +93,78 @@
   </si>
   <si>
     <t>Test 4</t>
+  </si>
+  <si>
+    <t>Test 5</t>
+  </si>
+  <si>
+    <t>Drink</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>Deaf</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Cow</t>
+  </si>
+  <si>
+    <t>Eat</t>
+  </si>
+  <si>
+    <t>Cry</t>
+  </si>
+  <si>
+    <t>Egg</t>
+  </si>
+  <si>
+    <t>Cup</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>cow</t>
+  </si>
+  <si>
+    <t>eat</t>
+  </si>
+  <si>
+    <t>cry</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>cup</t>
+  </si>
+  <si>
+    <t>computer</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>Test 6</t>
+  </si>
+  <si>
+    <t>drink</t>
+  </si>
+  <si>
+    <t>deaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drive </t>
+  </si>
+  <si>
+    <t xml:space="preserve">computer </t>
+  </si>
+  <si>
+    <t>Test 7</t>
   </si>
 </sst>
 </file>
@@ -116,15 +188,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -132,16 +210,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -435,12 +582,29 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -467,34 +631,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -514,6 +650,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="medium">
           <color indexed="64"/>
@@ -529,6 +673,9 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -543,12 +690,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DD2ABC0D-50C1-49C4-8D3A-5CA063F1F218}" name="Table5" displayName="Table5" ref="A2:D12" headerRowCount="0" totalsRowShown="0" dataDxfId="34" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DD2ABC0D-50C1-49C4-8D3A-5CA063F1F218}" name="Table5" displayName="Table5" ref="A2:D12" headerRowCount="0" totalsRowShown="0" dataDxfId="39" tableBorderDxfId="38">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F400AB7F-4E8B-4125-9E25-5ED9FB65B14F}" name="Column1" headerRowDxfId="30" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{3F22CA1A-5693-4313-92A4-EE54C2FDC4CF}" name="Test 1" headerRowDxfId="31" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{788734D9-F3D0-4322-87BC-6A1CAF964241}" name="Column2" headerRowDxfId="32" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{4FC0C234-7164-459C-8403-515A895D477E}" name="Column3" headerRowDxfId="33" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{F400AB7F-4E8B-4125-9E25-5ED9FB65B14F}" name="Column1" headerRowDxfId="37" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{3F22CA1A-5693-4313-92A4-EE54C2FDC4CF}" name="Test 1" headerRowDxfId="35" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{788734D9-F3D0-4322-87BC-6A1CAF964241}" name="Column2" headerRowDxfId="33" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{4FC0C234-7164-459C-8403-515A895D477E}" name="Column3" headerRowDxfId="31" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -907,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBF13E0-78B5-4465-B2C7-E04C9FCCA561}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1512,6 +1659,807 @@
       </c>
       <c r="D52" s="2"/>
     </row>
+    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C54" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58">
+        <v>0.59</v>
+      </c>
+      <c r="D58">
+        <v>9.7199999999999995E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <v>0.89490000000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62">
+        <v>0.93110000000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <v>0.39179999999999998</v>
+      </c>
+      <c r="D63">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64">
+        <v>0.69650000000000001</v>
+      </c>
+      <c r="D64">
+        <v>1.6000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65">
+        <v>0.30070000000000002</v>
+      </c>
+      <c r="D65">
+        <v>0.14599999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66">
+        <v>0.96150000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67">
+        <v>0.54090000000000005</v>
+      </c>
+      <c r="D67">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68">
+        <v>0.70489999999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B69" t="s">
+        <v>30</v>
+      </c>
+      <c r="C69">
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B70" t="s">
+        <v>31</v>
+      </c>
+      <c r="C70">
+        <v>0.44090000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="D71">
+        <v>0.1142</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72">
+        <v>0.37059999999999998</v>
+      </c>
+      <c r="D72">
+        <v>0.20799999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B73" t="s">
+        <v>33</v>
+      </c>
+      <c r="C73">
+        <v>0.75690000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B74" t="s">
+        <v>36</v>
+      </c>
+      <c r="C74">
+        <v>0.62090000000000001</v>
+      </c>
+      <c r="D74">
+        <v>7.8100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" t="s">
+        <v>35</v>
+      </c>
+      <c r="C75">
+        <v>0.95609999999999995</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C77" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79">
+        <v>0.91810000000000003</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>38</v>
+      </c>
+      <c r="C80">
+        <v>0.98219999999999996</v>
+      </c>
+      <c r="D80">
+        <v>4.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B81" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81">
+        <v>0.98319999999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83">
+        <v>0.7369</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>0.98450000000000004</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B85" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85">
+        <v>0.97040000000000004</v>
+      </c>
+      <c r="D85">
+        <v>5.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86">
+        <v>0.99</v>
+      </c>
+      <c r="D86">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87">
+        <v>0.52480000000000004</v>
+      </c>
+      <c r="D87">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B88" t="s">
+        <v>36</v>
+      </c>
+      <c r="C88">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="D88">
+        <v>2.35E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90">
+        <v>0.53220000000000001</v>
+      </c>
+      <c r="D90">
+        <v>2.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" t="s">
+        <v>13</v>
+      </c>
+      <c r="C91">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="D91">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92" t="s">
+        <v>30</v>
+      </c>
+      <c r="C92">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B93" t="s">
+        <v>31</v>
+      </c>
+      <c r="C93">
+        <v>0.95699999999999996</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B94" t="s">
+        <v>32</v>
+      </c>
+      <c r="C94">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" t="s">
+        <v>40</v>
+      </c>
+      <c r="C95">
+        <v>0.96879999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B96" t="s">
+        <v>33</v>
+      </c>
+      <c r="C96">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B97" t="s">
+        <v>34</v>
+      </c>
+      <c r="C97">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B98" t="s">
+        <v>41</v>
+      </c>
+      <c r="C98">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C100" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" t="s">
+        <v>33</v>
+      </c>
+      <c r="C102">
+        <v>0.99</v>
+      </c>
+      <c r="D102">
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B103" t="s">
+        <v>38</v>
+      </c>
+      <c r="C103">
+        <v>0.96640000000000004</v>
+      </c>
+      <c r="D103">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B104" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104">
+        <v>0.8306</v>
+      </c>
+      <c r="D104">
+        <v>5.7700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105" t="s">
+        <v>8</v>
+      </c>
+      <c r="C105">
+        <v>0.98109999999999997</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B106" t="s">
+        <v>6</v>
+      </c>
+      <c r="C106">
+        <v>0.68989999999999996</v>
+      </c>
+      <c r="D106">
+        <v>0.161</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B107" t="s">
+        <v>10</v>
+      </c>
+      <c r="C107">
+        <v>0.81899999999999995</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>0.90110000000000001</v>
+      </c>
+      <c r="D108">
+        <v>8.0699999999999994E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B109" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109">
+        <v>0.66439999999999999</v>
+      </c>
+      <c r="D109">
+        <v>5.9700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B110" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110">
+        <v>0.40649999999999997</v>
+      </c>
+      <c r="D110">
+        <v>0.19420000000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111" t="s">
+        <v>10</v>
+      </c>
+      <c r="C111">
+        <v>0.60840000000000005</v>
+      </c>
+      <c r="D111">
+        <v>1.4800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B112" t="s">
+        <v>38</v>
+      </c>
+      <c r="C112">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B113" t="s">
+        <v>10</v>
+      </c>
+      <c r="C113">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" t="s">
+        <v>38</v>
+      </c>
+      <c r="C114">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B115" t="s">
+        <v>30</v>
+      </c>
+      <c r="C115">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B116" t="s">
+        <v>38</v>
+      </c>
+      <c r="C116">
+        <v>0.78129999999999999</v>
+      </c>
+      <c r="D116">
+        <v>0.14829999999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117" t="s">
+        <v>38</v>
+      </c>
+      <c r="C117">
+        <v>0.51390000000000002</v>
+      </c>
+      <c r="D117">
+        <v>0.38869999999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118">
+        <v>0.90780000000000005</v>
+      </c>
+      <c r="D118">
+        <v>5.2900000000000003E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B119" t="s">
+        <v>38</v>
+      </c>
+      <c r="C119">
+        <v>0.80269999999999997</v>
+      </c>
+      <c r="D119">
+        <v>3.0099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B120" t="s">
+        <v>39</v>
+      </c>
+      <c r="C120">
+        <v>0.52</v>
+      </c>
+      <c r="D120">
+        <v>8.0999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B121" t="s">
+        <v>41</v>
+      </c>
+      <c r="C121">
+        <v>0.99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="4">

</xml_diff>

<commit_message>
97 % accuracy for models using own dataset
</commit_message>
<xml_diff>
--- a/translate/record of results.xlsx
+++ b/translate/record of results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\COS301\Hands-Up\translate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE64FEAA-B054-4002-A60D-E39A4FFAA788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFC94C9-EA76-4E10-AEF4-38B47A03867E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11088" yWindow="552" windowWidth="8688" windowHeight="8880" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="49">
   <si>
     <t>sign</t>
   </si>
@@ -165,6 +165,24 @@
   </si>
   <si>
     <t>Test 7</t>
+  </si>
+  <si>
+    <t>predicted</t>
+  </si>
+  <si>
+    <t>drive</t>
+  </si>
+  <si>
+    <t>same model different day</t>
+  </si>
+  <si>
+    <t>same model but trained again without any changes</t>
+  </si>
+  <si>
+    <t>(0.5 test accurcacy)</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1054,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBF13E0-78B5-4465-B2C7-E04C9FCCA561}">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="E202" sqref="E202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2192,7 +2210,7 @@
         <v>0</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>3</v>
@@ -2458,6 +2476,1048 @@
       </c>
       <c r="C121">
         <v>0.99</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C122" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D123" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" t="s">
+        <v>33</v>
+      </c>
+      <c r="C124">
+        <v>0.95950000000000002</v>
+      </c>
+      <c r="D124">
+        <v>6.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B125" t="s">
+        <v>38</v>
+      </c>
+      <c r="C125">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="D125">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126">
+        <v>0.61380000000000001</v>
+      </c>
+      <c r="D126">
+        <v>0.15820000000000001</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B127" t="s">
+        <v>8</v>
+      </c>
+      <c r="C127">
+        <v>0.96440000000000003</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B128" t="s">
+        <v>30</v>
+      </c>
+      <c r="C128">
+        <v>0.69240000000000002</v>
+      </c>
+      <c r="D128">
+        <v>0.2379</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B129" t="s">
+        <v>10</v>
+      </c>
+      <c r="C129">
+        <v>0.76780000000000004</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B130" t="s">
+        <v>10</v>
+      </c>
+      <c r="C130">
+        <v>0.95179999999999998</v>
+      </c>
+      <c r="D130">
+        <v>3.0800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B131" t="s">
+        <v>30</v>
+      </c>
+      <c r="C131">
+        <v>0.80969999999999998</v>
+      </c>
+      <c r="D131">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B132" t="s">
+        <v>6</v>
+      </c>
+      <c r="C132">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="D132">
+        <v>1.6000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B133" t="s">
+        <v>10</v>
+      </c>
+      <c r="C133">
+        <v>0.74609999999999999</v>
+      </c>
+      <c r="D133">
+        <v>0.12620000000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B134" t="s">
+        <v>38</v>
+      </c>
+      <c r="C134">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B135" t="s">
+        <v>15</v>
+      </c>
+      <c r="C135">
+        <v>0.55010000000000003</v>
+      </c>
+      <c r="D135">
+        <v>6.3799999999999996E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B136" t="s">
+        <v>36</v>
+      </c>
+      <c r="C136">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B137" t="s">
+        <v>30</v>
+      </c>
+      <c r="C137">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B138" t="s">
+        <v>38</v>
+      </c>
+      <c r="C138">
+        <v>0.99</v>
+      </c>
+      <c r="D138">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B139" t="s">
+        <v>38</v>
+      </c>
+      <c r="C139">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="D139">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B140" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140">
+        <v>0.73660000000000003</v>
+      </c>
+      <c r="D140">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B141" t="s">
+        <v>8</v>
+      </c>
+      <c r="C141">
+        <v>0.97760000000000002</v>
+      </c>
+      <c r="D141">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B142" t="s">
+        <v>38</v>
+      </c>
+      <c r="C142">
+        <v>0.99409999999999998</v>
+      </c>
+      <c r="D142">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B143" t="s">
+        <v>35</v>
+      </c>
+      <c r="C143">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C145" t="s">
+        <v>46</v>
+      </c>
+      <c r="E145" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A146" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C146" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D146" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A147" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B147" t="s">
+        <v>33</v>
+      </c>
+      <c r="C147">
+        <v>0.96</v>
+      </c>
+      <c r="D147">
+        <v>2.0899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A148" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B148" t="s">
+        <v>38</v>
+      </c>
+      <c r="C148">
+        <v>0.96779999999999999</v>
+      </c>
+      <c r="D148">
+        <v>6.3E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A149" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B149" t="s">
+        <v>7</v>
+      </c>
+      <c r="C149">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A150" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B150" t="s">
+        <v>8</v>
+      </c>
+      <c r="C150">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A151" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B151" t="s">
+        <v>30</v>
+      </c>
+      <c r="C151">
+        <v>0.59630000000000005</v>
+      </c>
+      <c r="D151">
+        <v>6.9500000000000006E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A152" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B152" t="s">
+        <v>10</v>
+      </c>
+      <c r="C152">
+        <v>0.96299999999999997</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A153" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B153" t="s">
+        <v>10</v>
+      </c>
+      <c r="C153">
+        <v>0.55830000000000002</v>
+      </c>
+      <c r="D153">
+        <v>0.3548</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A154" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B154" t="s">
+        <v>35</v>
+      </c>
+      <c r="C154">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="D154">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A155" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B155" t="s">
+        <v>33</v>
+      </c>
+      <c r="C155">
+        <v>0.79530000000000001</v>
+      </c>
+      <c r="D155">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B156" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156">
+        <v>0.88</v>
+      </c>
+      <c r="D156">
+        <v>1.8599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A157" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B157" t="s">
+        <v>38</v>
+      </c>
+      <c r="C157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A158" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B158" t="s">
+        <v>15</v>
+      </c>
+      <c r="C158">
+        <v>0.87139999999999995</v>
+      </c>
+      <c r="D158">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A159" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B159" t="s">
+        <v>36</v>
+      </c>
+      <c r="C159">
+        <v>0.63790000000000002</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A160" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B160" t="s">
+        <v>30</v>
+      </c>
+      <c r="C160">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B161" t="s">
+        <v>38</v>
+      </c>
+      <c r="C161">
+        <v>0.82550000000000001</v>
+      </c>
+      <c r="D161">
+        <v>5.1799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B162" t="s">
+        <v>12</v>
+      </c>
+      <c r="C162">
+        <v>0.34279999999999999</v>
+      </c>
+      <c r="D162">
+        <v>0.1578</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B163" t="s">
+        <v>14</v>
+      </c>
+      <c r="C163">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="D163">
+        <v>0.34710000000000002</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B164" t="s">
+        <v>33</v>
+      </c>
+      <c r="C164">
+        <v>0.81869999999999998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B165" t="s">
+        <v>8</v>
+      </c>
+      <c r="C165">
+        <v>0.53249999999999997</v>
+      </c>
+      <c r="D165">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D167">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A168" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B168" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C168" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D168" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" t="s">
+        <v>5</v>
+      </c>
+      <c r="C169">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B170" t="s">
+        <v>38</v>
+      </c>
+      <c r="C170">
+        <v>0.83609999999999995</v>
+      </c>
+      <c r="D170">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B171" t="s">
+        <v>31</v>
+      </c>
+      <c r="C171">
+        <v>0.91879999999999995</v>
+      </c>
+      <c r="D171">
+        <v>6.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B172" t="s">
+        <v>8</v>
+      </c>
+      <c r="C172">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B173" t="s">
+        <v>38</v>
+      </c>
+      <c r="C173">
+        <v>0.5927</v>
+      </c>
+      <c r="D173">
+        <v>3.7499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B174" t="s">
+        <v>15</v>
+      </c>
+      <c r="C174">
+        <v>0.72</v>
+      </c>
+      <c r="D174">
+        <v>4.7800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A175" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B175" t="s">
+        <v>15</v>
+      </c>
+      <c r="C175">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A176" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B176" t="s">
+        <v>38</v>
+      </c>
+      <c r="C176">
+        <v>0.57340000000000002</v>
+      </c>
+      <c r="D176">
+        <v>0.1973</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A177" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B177" t="s">
+        <v>36</v>
+      </c>
+      <c r="C177">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="D177">
+        <v>5.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A178" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B178" t="s">
+        <v>38</v>
+      </c>
+      <c r="C178">
+        <v>0.59150000000000003</v>
+      </c>
+      <c r="D178">
+        <v>2.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A179" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B179" t="s">
+        <v>38</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B180" t="s">
+        <v>31</v>
+      </c>
+      <c r="C180">
+        <v>0.64770000000000005</v>
+      </c>
+      <c r="D180">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B181" t="s">
+        <v>38</v>
+      </c>
+      <c r="C181">
+        <v>0.98</v>
+      </c>
+      <c r="D181">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B182" t="s">
+        <v>30</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A183" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B183" t="s">
+        <v>38</v>
+      </c>
+      <c r="C183">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D183">
+        <v>0.4632</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B184" t="s">
+        <v>32</v>
+      </c>
+      <c r="C184">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B185" t="s">
+        <v>12</v>
+      </c>
+      <c r="C185">
+        <v>0.51819999999999999</v>
+      </c>
+      <c r="D185">
+        <v>0.21609999999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B186" t="s">
+        <v>33</v>
+      </c>
+      <c r="C186">
+        <v>0.92949999999999999</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B187" t="s">
+        <v>34</v>
+      </c>
+      <c r="C187">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A188" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B190" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C190" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D190" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B191" t="s">
+        <v>5</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A192" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B192" t="s">
+        <v>6</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B193" t="s">
+        <v>7</v>
+      </c>
+      <c r="C193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B194" t="s">
+        <v>8</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A195" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B195" t="s">
+        <v>9</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B196" t="s">
+        <v>10</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B197" t="s">
+        <v>15</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B198" t="s">
+        <v>12</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A199" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B199" t="s">
+        <v>14</v>
+      </c>
+      <c r="C199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A200" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B200" t="s">
+        <v>13</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A201" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A202" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B202" t="s">
+        <v>39</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+      <c r="E202" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A203" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B203" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A204" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A205" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B205" t="s">
+        <v>31</v>
+      </c>
+      <c r="C205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A206" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B206" t="s">
+        <v>32</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A207" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B207" t="s">
+        <v>44</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A208" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B208" t="s">
+        <v>33</v>
+      </c>
+      <c r="C208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A209" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B209" t="s">
+        <v>34</v>
+      </c>
+      <c r="C209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A210" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more words into the dataset
</commit_message>
<xml_diff>
--- a/translate/record of results.xlsx
+++ b/translate/record of results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\COS301\Hands-Up\translate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFC94C9-EA76-4E10-AEF4-38B47A03867E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B480BE5-8A58-4CCB-97EE-739C345C9060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
+    <workbookView xWindow="11664" yWindow="240" windowWidth="8688" windowHeight="8880" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="48">
   <si>
     <t>sign</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>(0.5 test accurcacy)</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBF13E0-78B5-4465-B2C7-E04C9FCCA561}">
-  <dimension ref="A1:E210"/>
+  <dimension ref="A1:E232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="E202" sqref="E202"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="D227" sqref="D227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3340,7 +3337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="3" t="s">
         <v>7</v>
       </c>
@@ -3351,7 +3348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="4" t="s">
         <v>8</v>
       </c>
@@ -3362,7 +3359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="3" t="s">
         <v>9</v>
       </c>
@@ -3373,7 +3370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="4" t="s">
         <v>10</v>
       </c>
@@ -3384,7 +3381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="3" t="s">
         <v>11</v>
       </c>
@@ -3395,7 +3392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="4" t="s">
         <v>12</v>
       </c>
@@ -3406,7 +3403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="3" t="s">
         <v>14</v>
       </c>
@@ -3417,7 +3414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A200" s="5" t="s">
         <v>13</v>
       </c>
@@ -3428,12 +3425,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="4" t="s">
         <v>22</v>
       </c>
@@ -3443,11 +3440,8 @@
       <c r="C202">
         <v>1</v>
       </c>
-      <c r="E202" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="3" t="s">
         <v>23</v>
       </c>
@@ -3455,12 +3449,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="3" t="s">
         <v>25</v>
       </c>
@@ -3471,7 +3465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="4" t="s">
         <v>26</v>
       </c>
@@ -3482,7 +3476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="3" t="s">
         <v>21</v>
       </c>
@@ -3493,7 +3487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="4" t="s">
         <v>27</v>
       </c>
@@ -3504,7 +3498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="3" t="s">
         <v>28</v>
       </c>
@@ -3515,9 +3509,256 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="4" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A212" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B212" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C212" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D212" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A213" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B213" t="s">
+        <v>5</v>
+      </c>
+      <c r="C213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A214" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B214" t="s">
+        <v>6</v>
+      </c>
+      <c r="C214">
+        <v>0.9365</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B215" t="s">
+        <v>7</v>
+      </c>
+      <c r="C215">
+        <v>0.94920000000000004</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B216" t="s">
+        <v>8</v>
+      </c>
+      <c r="C216">
+        <v>0.99739999999999995</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B217" t="s">
+        <v>9</v>
+      </c>
+      <c r="C217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B218" t="s">
+        <v>10</v>
+      </c>
+      <c r="C218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B219" t="s">
+        <v>15</v>
+      </c>
+      <c r="C219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A220" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B220" t="s">
+        <v>12</v>
+      </c>
+      <c r="C220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A221" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B221" t="s">
+        <v>14</v>
+      </c>
+      <c r="C221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A222" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B222" t="s">
+        <v>13</v>
+      </c>
+      <c r="C222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A223" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B223" t="s">
+        <v>9</v>
+      </c>
+      <c r="C223">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="D223">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B224" t="s">
+        <v>22</v>
+      </c>
+      <c r="C224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B225" t="s">
+        <v>23</v>
+      </c>
+      <c r="C225">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A226" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B226" t="s">
+        <v>12</v>
+      </c>
+      <c r="C226">
+        <v>0.99839999999999995</v>
+      </c>
+      <c r="D226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B227" t="s">
+        <v>25</v>
+      </c>
+      <c r="C227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B228" t="s">
+        <v>26</v>
+      </c>
+      <c r="C228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B229" t="s">
+        <v>21</v>
+      </c>
+      <c r="C229">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A230" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B230" t="s">
+        <v>5</v>
+      </c>
+      <c r="C230">
+        <v>0.99780000000000002</v>
+      </c>
+      <c r="D230">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B231" t="s">
+        <v>28</v>
+      </c>
+      <c r="C231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B232" t="s">
+        <v>15</v>
+      </c>
+      <c r="C232">
+        <v>0.83340000000000003</v>
+      </c>
+      <c r="D232">
+        <v>5.2600000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Model working for 30 words with one or two changes
</commit_message>
<xml_diff>
--- a/translate/record of results.xlsx
+++ b/translate/record of results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\COS301\Hands-Up\translate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B480BE5-8A58-4CCB-97EE-739C345C9060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D91595-5CC4-4DD3-AE22-30D48E55B7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11664" yWindow="240" windowWidth="8688" windowHeight="8880" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
+    <workbookView xWindow="11820" yWindow="0" windowWidth="8688" windowHeight="12336" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="59">
   <si>
     <t>sign</t>
   </si>
@@ -180,6 +180,39 @@
   </si>
   <si>
     <t>(0.5 test accurcacy)</t>
+  </si>
+  <si>
+    <t>feel</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>father</t>
+  </si>
+  <si>
+    <t>full</t>
+  </si>
+  <si>
+    <t>future</t>
+  </si>
+  <si>
+    <t>girl</t>
+  </si>
+  <si>
+    <t>give</t>
+  </si>
+  <si>
+    <t>go</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>grandma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">future </t>
   </si>
 </sst>
 </file>
@@ -280,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,12 +339,148 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
+  <dxfs count="44">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -323,18 +492,12 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -361,25 +524,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -404,12 +548,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -418,18 +556,12 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -456,25 +588,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -499,12 +612,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -513,18 +620,12 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -551,25 +652,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -594,12 +676,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -608,18 +684,12 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -646,25 +716,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -688,9 +739,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -705,48 +753,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DD2ABC0D-50C1-49C4-8D3A-5CA063F1F218}" name="Table5" displayName="Table5" ref="A2:D12" headerRowCount="0" totalsRowShown="0" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DD2ABC0D-50C1-49C4-8D3A-5CA063F1F218}" name="Table5" displayName="Table5" ref="A2:D12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="43">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F400AB7F-4E8B-4125-9E25-5ED9FB65B14F}" name="Column1" headerRowDxfId="37" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{3F22CA1A-5693-4313-92A4-EE54C2FDC4CF}" name="Test 1" headerRowDxfId="35" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{788734D9-F3D0-4322-87BC-6A1CAF964241}" name="Column2" headerRowDxfId="33" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{4FC0C234-7164-459C-8403-515A895D477E}" name="Column3" headerRowDxfId="31" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{F400AB7F-4E8B-4125-9E25-5ED9FB65B14F}" name="Column1" headerRowDxfId="42" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{3F22CA1A-5693-4313-92A4-EE54C2FDC4CF}" name="Test 1" headerRowDxfId="41" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{788734D9-F3D0-4322-87BC-6A1CAF964241}" name="Column2" headerRowDxfId="40" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{4FC0C234-7164-459C-8403-515A895D477E}" name="Column3" headerRowDxfId="39" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E569A974-8B60-4556-8570-6A44C4FBD727}" name="Table57" displayName="Table57" ref="A16:D26" headerRowCount="0" totalsRowShown="0" dataDxfId="29" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E569A974-8B60-4556-8570-6A44C4FBD727}" name="Table57" displayName="Table57" ref="A16:D26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="38">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8766D2EA-8EEA-45A1-8B07-7FA7D5ACC38E}" name="Column1" headerRowDxfId="27" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{A099EBA9-F36A-46FA-BDB1-F7CAF089E494}" name="Test 1" headerRowDxfId="25" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{92A9AE78-3CB8-4AAA-8266-990E00ABEE53}" name="Column2" headerRowDxfId="23" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{8468543C-F567-482E-BE69-7F793167F224}" name="Column3" headerRowDxfId="21" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{8766D2EA-8EEA-45A1-8B07-7FA7D5ACC38E}" name="Column1" headerRowDxfId="37" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{A099EBA9-F36A-46FA-BDB1-F7CAF089E494}" name="Test 1" headerRowDxfId="36" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{92A9AE78-3CB8-4AAA-8266-990E00ABEE53}" name="Column2" headerRowDxfId="35" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{8468543C-F567-482E-BE69-7F793167F224}" name="Column3" headerRowDxfId="34" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1C6A1CC9-8976-4B5C-B94C-E8A89F240FFB}" name="Table578" displayName="Table578" ref="A29:D39" headerRowCount="0" totalsRowShown="0" dataDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1C6A1CC9-8976-4B5C-B94C-E8A89F240FFB}" name="Table578" displayName="Table578" ref="A29:D39" headerRowCount="0" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="33">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E504D3A5-FC9A-45F6-8C0E-D7A50AF19A75}" name="Column1" headerRowDxfId="17" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{6EAF6B0D-E32F-4ABE-93B4-E394AE2A7E61}" name="Test 1" headerRowDxfId="15" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{8BDDF0B1-E9A5-48D4-B164-ADE5E3372319}" name="Column2" headerRowDxfId="13" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{CD0DB33E-E98F-4D80-969C-C6CB71E17312}" name="Column3" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{E504D3A5-FC9A-45F6-8C0E-D7A50AF19A75}" name="Column1" headerRowDxfId="32" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{6EAF6B0D-E32F-4ABE-93B4-E394AE2A7E61}" name="Test 1" headerRowDxfId="31" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{8BDDF0B1-E9A5-48D4-B164-ADE5E3372319}" name="Column2" headerRowDxfId="30" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{CD0DB33E-E98F-4D80-969C-C6CB71E17312}" name="Column3" headerRowDxfId="29" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{2B773CE3-EB5B-45E6-9DCA-44D0A01FB542}" name="Table5789" displayName="Table5789" ref="A42:D52" headerRowCount="0" totalsRowShown="0" dataDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{2B773CE3-EB5B-45E6-9DCA-44D0A01FB542}" name="Table5789" displayName="Table5789" ref="A42:D52" headerRowCount="0" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" tableBorderDxfId="28">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DC2E491C-2CD4-4E89-AC71-91DE1A7E1452}" name="Column1" headerRowDxfId="7" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{BE664661-355B-4988-923D-8558A307F1DC}" name="Test 1" headerRowDxfId="5" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{E149DA85-C608-4816-AFAC-5502546D39B6}" name="Column2" headerRowDxfId="3" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{0BD5DA97-7603-4D27-9BC6-3BFD8A154644}" name="Column3" headerRowDxfId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{DC2E491C-2CD4-4E89-AC71-91DE1A7E1452}" name="Column1" headerRowDxfId="27" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{BE664661-355B-4988-923D-8558A307F1DC}" name="Test 1" headerRowDxfId="26" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{E149DA85-C608-4816-AFAC-5502546D39B6}" name="Column2" headerRowDxfId="25" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{0BD5DA97-7603-4D27-9BC6-3BFD8A154644}" name="Column3" headerRowDxfId="24" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1069,21 +1117,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBF13E0-78B5-4465-B2C7-E04C9FCCA561}">
-  <dimension ref="A1:E232"/>
+  <dimension ref="A1:E264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
-      <selection activeCell="D227" sqref="D227"/>
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A235" sqref="A235:A264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1125,7 +1174,6 @@
       <c r="C4" s="2">
         <v>0.87009999999999998</v>
       </c>
-      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1240,7 +1288,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1282,7 +1330,6 @@
       <c r="C18" s="2">
         <v>1</v>
       </c>
-      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -1294,7 +1341,6 @@
       <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -1306,7 +1352,6 @@
       <c r="C20" s="2">
         <v>1</v>
       </c>
-      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -1374,7 +1419,6 @@
       <c r="C25" s="2">
         <v>0.99929999999999997</v>
       </c>
-      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -1391,7 +1435,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1419,7 +1463,6 @@
       <c r="C30" s="2">
         <v>1</v>
       </c>
-      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
@@ -1459,7 +1502,6 @@
       <c r="C33" s="2">
         <v>0.84</v>
       </c>
-      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
@@ -1471,7 +1513,6 @@
       <c r="C34" s="2">
         <v>0.99</v>
       </c>
-      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
@@ -1483,7 +1524,6 @@
       <c r="C35" s="2">
         <v>1</v>
       </c>
-      <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
@@ -1495,7 +1535,6 @@
       <c r="C36" s="2">
         <v>1</v>
       </c>
-      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -1507,7 +1546,6 @@
       <c r="C37" s="2">
         <v>1</v>
       </c>
-      <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1519,7 +1557,6 @@
       <c r="C38" s="2">
         <v>0.81379999999999997</v>
       </c>
-      <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
@@ -1531,10 +1568,9 @@
       <c r="C39" s="2">
         <v>0.98</v>
       </c>
-      <c r="D39" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1562,7 +1598,6 @@
       <c r="C43" s="2">
         <v>0.97309999999999997</v>
       </c>
-      <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -1574,7 +1609,6 @@
       <c r="C44" s="2">
         <v>1</v>
       </c>
-      <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
@@ -1586,7 +1620,6 @@
       <c r="C45" s="2">
         <v>1</v>
       </c>
-      <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
@@ -1598,7 +1631,6 @@
       <c r="C46" s="2">
         <v>0.95289999999999997</v>
       </c>
-      <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
@@ -1610,7 +1642,6 @@
       <c r="C47" s="2">
         <v>0.98</v>
       </c>
-      <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
@@ -1622,7 +1653,6 @@
       <c r="C48" s="2">
         <v>0.91779999999999995</v>
       </c>
-      <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
@@ -1634,7 +1664,6 @@
       <c r="C49" s="2">
         <v>0.98150000000000004</v>
       </c>
-      <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
@@ -1646,7 +1675,6 @@
       <c r="C50" s="2">
         <v>0.96279999999999999</v>
       </c>
-      <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
@@ -1672,10 +1700,9 @@
       <c r="C52" s="2">
         <v>1</v>
       </c>
-      <c r="D52" s="2"/>
     </row>
     <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1697,10 +1724,10 @@
       <c r="A56" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="2">
         <v>0.76</v>
       </c>
     </row>
@@ -1708,10 +1735,10 @@
       <c r="A57" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="2">
         <v>0.86</v>
       </c>
     </row>
@@ -1719,13 +1746,13 @@
       <c r="A58" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="2">
         <v>0.59</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="2">
         <v>9.7199999999999995E-2</v>
       </c>
     </row>
@@ -1733,10 +1760,10 @@
       <c r="A59" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="2">
         <v>0.9</v>
       </c>
     </row>
@@ -1744,10 +1771,10 @@
       <c r="A60" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="2">
         <v>0.88</v>
       </c>
     </row>
@@ -1755,10 +1782,10 @@
       <c r="A61" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="2">
         <v>0.89490000000000003</v>
       </c>
     </row>
@@ -1766,10 +1793,10 @@
       <c r="A62" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="2">
         <v>0.93110000000000004</v>
       </c>
     </row>
@@ -1777,13 +1804,13 @@
       <c r="A63" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="2">
         <v>0.39179999999999998</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="2">
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
@@ -1791,13 +1818,13 @@
       <c r="A64" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="2">
         <v>0.69650000000000001</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="2">
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
@@ -1805,13 +1832,13 @@
       <c r="A65" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="2">
         <v>0.30070000000000002</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="2">
         <v>0.14599999999999999</v>
       </c>
     </row>
@@ -1819,10 +1846,10 @@
       <c r="A66" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="2">
         <v>0.96150000000000002</v>
       </c>
     </row>
@@ -1830,13 +1857,13 @@
       <c r="A67" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="2">
         <v>0.54090000000000005</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="2">
         <v>2.3999999999999998E-3</v>
       </c>
     </row>
@@ -1844,10 +1871,10 @@
       <c r="A68" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="2">
         <v>0.70489999999999997</v>
       </c>
     </row>
@@ -1855,10 +1882,10 @@
       <c r="A69" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="2">
         <v>0.92400000000000004</v>
       </c>
     </row>
@@ -1866,10 +1893,10 @@
       <c r="A70" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="2">
         <v>0.44090000000000001</v>
       </c>
     </row>
@@ -1877,13 +1904,13 @@
       <c r="A71" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="2">
         <v>0.63300000000000001</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="2">
         <v>0.1142</v>
       </c>
     </row>
@@ -1891,13 +1918,13 @@
       <c r="A72" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="2">
         <v>0.37059999999999998</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="2">
         <v>0.20799999999999999</v>
       </c>
     </row>
@@ -1905,10 +1932,10 @@
       <c r="A73" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="2">
         <v>0.75690000000000002</v>
       </c>
     </row>
@@ -1916,13 +1943,13 @@
       <c r="A74" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="2">
         <v>0.62090000000000001</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="2">
         <v>7.8100000000000003E-2</v>
       </c>
     </row>
@@ -1930,15 +1957,15 @@
       <c r="A75" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="2">
         <v>0.95609999999999995</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C77" t="s">
+      <c r="C77" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1960,10 +1987,10 @@
       <c r="A79" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="2">
         <v>0.91810000000000003</v>
       </c>
     </row>
@@ -1971,13 +1998,13 @@
       <c r="A80" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="2">
         <v>0.98219999999999996</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="2">
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
@@ -1985,10 +2012,10 @@
       <c r="A81" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="2">
         <v>0.98319999999999996</v>
       </c>
     </row>
@@ -1996,10 +2023,10 @@
       <c r="A82" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2007,10 +2034,10 @@
       <c r="A83" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="2">
         <v>0.7369</v>
       </c>
     </row>
@@ -2018,10 +2045,10 @@
       <c r="A84" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="2">
         <v>0.98450000000000004</v>
       </c>
     </row>
@@ -2029,13 +2056,13 @@
       <c r="A85" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="2">
         <v>0.97040000000000004</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="2">
         <v>5.1999999999999998E-3</v>
       </c>
     </row>
@@ -2043,13 +2070,13 @@
       <c r="A86" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="2">
         <v>0.99</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="2">
         <v>1E-4</v>
       </c>
     </row>
@@ -2057,13 +2084,13 @@
       <c r="A87" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="2">
         <v>0.52480000000000004</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="2">
         <v>1.9E-2</v>
       </c>
     </row>
@@ -2071,13 +2098,13 @@
       <c r="A88" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="2">
         <v>0.77900000000000003</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="2">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2085,10 +2112,10 @@
       <c r="A89" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="2">
         <v>0.99</v>
       </c>
     </row>
@@ -2096,13 +2123,13 @@
       <c r="A90" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="2">
         <v>0.53220000000000001</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="2">
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
@@ -2110,13 +2137,13 @@
       <c r="A91" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="2">
         <v>0.98799999999999999</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="2">
         <v>3.8E-3</v>
       </c>
     </row>
@@ -2124,10 +2151,10 @@
       <c r="A92" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="2">
         <v>0.99</v>
       </c>
     </row>
@@ -2135,10 +2162,10 @@
       <c r="A93" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="2">
         <v>0.95699999999999996</v>
       </c>
     </row>
@@ -2146,10 +2173,10 @@
       <c r="A94" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="2">
         <v>0.79</v>
       </c>
     </row>
@@ -2157,10 +2184,10 @@
       <c r="A95" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="2">
         <v>0.96879999999999999</v>
       </c>
     </row>
@@ -2168,10 +2195,10 @@
       <c r="A96" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="2">
         <v>0.71</v>
       </c>
     </row>
@@ -2179,10 +2206,10 @@
       <c r="A97" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="2">
         <v>0.84</v>
       </c>
     </row>
@@ -2190,15 +2217,15 @@
       <c r="A98" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="2">
         <v>0.92</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C100" t="s">
+      <c r="C100" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2220,13 +2247,13 @@
       <c r="A102" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="2">
         <v>0.99</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="2">
         <v>1.9E-3</v>
       </c>
     </row>
@@ -2234,13 +2261,13 @@
       <c r="A103" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="2">
         <v>0.96640000000000004</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="2">
         <v>1.5E-3</v>
       </c>
     </row>
@@ -2248,13 +2275,13 @@
       <c r="A104" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="2">
         <v>0.8306</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="2">
         <v>5.7700000000000001E-2</v>
       </c>
     </row>
@@ -2262,10 +2289,10 @@
       <c r="A105" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C105">
+      <c r="C105" s="2">
         <v>0.98109999999999997</v>
       </c>
     </row>
@@ -2273,13 +2300,13 @@
       <c r="A106" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="2">
         <v>0.68989999999999996</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="2">
         <v>0.161</v>
       </c>
     </row>
@@ -2287,10 +2314,10 @@
       <c r="A107" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="2">
         <v>0.81899999999999995</v>
       </c>
     </row>
@@ -2298,13 +2325,13 @@
       <c r="A108" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="2">
         <v>0.90110000000000001</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="2">
         <v>8.0699999999999994E-2</v>
       </c>
     </row>
@@ -2312,13 +2339,13 @@
       <c r="A109" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="2">
         <v>0.66439999999999999</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="2">
         <v>5.9700000000000003E-2</v>
       </c>
     </row>
@@ -2326,13 +2353,13 @@
       <c r="A110" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C110">
+      <c r="C110" s="2">
         <v>0.40649999999999997</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="2">
         <v>0.19420000000000001</v>
       </c>
     </row>
@@ -2340,13 +2367,13 @@
       <c r="A111" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C111">
+      <c r="C111" s="2">
         <v>0.60840000000000005</v>
       </c>
-      <c r="D111">
+      <c r="D111" s="2">
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
@@ -2354,10 +2381,10 @@
       <c r="A112" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="2">
         <v>0.9</v>
       </c>
     </row>
@@ -2365,10 +2392,10 @@
       <c r="A113" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="2">
         <v>0.75</v>
       </c>
     </row>
@@ -2376,10 +2403,10 @@
       <c r="A114" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="2">
         <v>0.55300000000000005</v>
       </c>
     </row>
@@ -2387,10 +2414,10 @@
       <c r="A115" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="2">
         <v>0.99</v>
       </c>
     </row>
@@ -2398,13 +2425,13 @@
       <c r="A116" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="2">
         <v>0.78129999999999999</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="2">
         <v>0.14829999999999999</v>
       </c>
     </row>
@@ -2412,13 +2439,13 @@
       <c r="A117" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="2">
         <v>0.51390000000000002</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="2">
         <v>0.38869999999999999</v>
       </c>
     </row>
@@ -2426,13 +2453,13 @@
       <c r="A118" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C118">
+      <c r="C118" s="2">
         <v>0.90780000000000005</v>
       </c>
-      <c r="D118">
+      <c r="D118" s="2">
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
@@ -2440,13 +2467,13 @@
       <c r="A119" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C119">
+      <c r="C119" s="2">
         <v>0.80269999999999997</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="2">
         <v>3.0099999999999998E-2</v>
       </c>
     </row>
@@ -2454,13 +2481,13 @@
       <c r="A120" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C120">
+      <c r="C120" s="2">
         <v>0.52</v>
       </c>
-      <c r="D120">
+      <c r="D120" s="2">
         <v>8.0999999999999996E-3</v>
       </c>
     </row>
@@ -2468,15 +2495,15 @@
       <c r="A121" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C121">
+      <c r="C121" s="2">
         <v>0.99</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C122" t="s">
+      <c r="C122" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2498,13 +2525,13 @@
       <c r="A124" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C124">
+      <c r="C124" s="2">
         <v>0.95950000000000002</v>
       </c>
-      <c r="D124">
+      <c r="D124" s="2">
         <v>6.7000000000000002E-3</v>
       </c>
     </row>
@@ -2512,13 +2539,13 @@
       <c r="A125" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C125">
+      <c r="C125" s="2">
         <v>0.92500000000000004</v>
       </c>
-      <c r="D125">
+      <c r="D125" s="2">
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
@@ -2526,13 +2553,13 @@
       <c r="A126" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="2">
         <v>0.61380000000000001</v>
       </c>
-      <c r="D126">
+      <c r="D126" s="2">
         <v>0.15820000000000001</v>
       </c>
     </row>
@@ -2540,10 +2567,10 @@
       <c r="A127" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C127">
+      <c r="C127" s="2">
         <v>0.96440000000000003</v>
       </c>
     </row>
@@ -2551,13 +2578,13 @@
       <c r="A128" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C128">
+      <c r="C128" s="2">
         <v>0.69240000000000002</v>
       </c>
-      <c r="D128">
+      <c r="D128" s="2">
         <v>0.2379</v>
       </c>
     </row>
@@ -2565,10 +2592,10 @@
       <c r="A129" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="2">
         <v>0.76780000000000004</v>
       </c>
     </row>
@@ -2576,13 +2603,13 @@
       <c r="A130" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C130">
+      <c r="C130" s="2">
         <v>0.95179999999999998</v>
       </c>
-      <c r="D130">
+      <c r="D130" s="2">
         <v>3.0800000000000001E-2</v>
       </c>
     </row>
@@ -2590,13 +2617,13 @@
       <c r="A131" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C131">
+      <c r="C131" s="2">
         <v>0.80969999999999998</v>
       </c>
-      <c r="D131">
+      <c r="D131" s="2">
         <v>0.8</v>
       </c>
     </row>
@@ -2604,13 +2631,13 @@
       <c r="A132" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C132">
+      <c r="C132" s="2">
         <v>0.88300000000000001</v>
       </c>
-      <c r="D132">
+      <c r="D132" s="2">
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
@@ -2618,13 +2645,13 @@
       <c r="A133" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C133">
+      <c r="C133" s="2">
         <v>0.74609999999999999</v>
       </c>
-      <c r="D133">
+      <c r="D133" s="2">
         <v>0.12620000000000001</v>
       </c>
     </row>
@@ -2632,10 +2659,10 @@
       <c r="A134" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C134">
+      <c r="C134" s="2">
         <v>0.99</v>
       </c>
     </row>
@@ -2643,13 +2670,13 @@
       <c r="A135" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C135">
+      <c r="C135" s="2">
         <v>0.55010000000000003</v>
       </c>
-      <c r="D135">
+      <c r="D135" s="2">
         <v>6.3799999999999996E-2</v>
       </c>
     </row>
@@ -2657,10 +2684,10 @@
       <c r="A136" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C136">
+      <c r="C136" s="2">
         <v>0.74</v>
       </c>
     </row>
@@ -2668,10 +2695,10 @@
       <c r="A137" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C137">
+      <c r="C137" s="2">
         <v>0.98</v>
       </c>
     </row>
@@ -2679,13 +2706,13 @@
       <c r="A138" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C138">
+      <c r="C138" s="2">
         <v>0.99</v>
       </c>
-      <c r="D138">
+      <c r="D138" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
@@ -2693,13 +2720,13 @@
       <c r="A139" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C139">
+      <c r="C139" s="2">
         <v>0.98399999999999999</v>
       </c>
-      <c r="D139">
+      <c r="D139" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
@@ -2707,13 +2734,13 @@
       <c r="A140" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="2">
         <v>0.73660000000000003</v>
       </c>
-      <c r="D140">
+      <c r="D140" s="2">
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
@@ -2721,13 +2748,13 @@
       <c r="A141" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C141">
+      <c r="C141" s="2">
         <v>0.97760000000000002</v>
       </c>
-      <c r="D141">
+      <c r="D141" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
@@ -2735,13 +2762,13 @@
       <c r="A142" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C142">
+      <c r="C142" s="2">
         <v>0.99409999999999998</v>
       </c>
-      <c r="D142">
+      <c r="D142" s="2">
         <v>1E-4</v>
       </c>
     </row>
@@ -2749,18 +2776,18 @@
       <c r="A143" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C143">
+      <c r="C143" s="2">
         <v>0.98</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C145" t="s">
+      <c r="C145" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E145" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2782,13 +2809,13 @@
       <c r="A147" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C147">
+      <c r="C147" s="2">
         <v>0.96</v>
       </c>
-      <c r="D147">
+      <c r="D147" s="2">
         <v>2.0899999999999998E-2</v>
       </c>
     </row>
@@ -2796,13 +2823,13 @@
       <c r="A148" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C148">
+      <c r="C148" s="2">
         <v>0.96779999999999999</v>
       </c>
-      <c r="D148">
+      <c r="D148" s="2">
         <v>6.3E-3</v>
       </c>
     </row>
@@ -2810,10 +2837,10 @@
       <c r="A149" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C149">
+      <c r="C149" s="2">
         <v>0.67</v>
       </c>
     </row>
@@ -2821,10 +2848,10 @@
       <c r="A150" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C150">
+      <c r="C150" s="2">
         <v>0.54</v>
       </c>
     </row>
@@ -2832,13 +2859,13 @@
       <c r="A151" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C151">
+      <c r="C151" s="2">
         <v>0.59630000000000005</v>
       </c>
-      <c r="D151">
+      <c r="D151" s="2">
         <v>6.9500000000000006E-2</v>
       </c>
     </row>
@@ -2846,10 +2873,10 @@
       <c r="A152" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C152">
+      <c r="C152" s="2">
         <v>0.96299999999999997</v>
       </c>
     </row>
@@ -2857,13 +2884,13 @@
       <c r="A153" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C153">
+      <c r="C153" s="2">
         <v>0.55830000000000002</v>
       </c>
-      <c r="D153">
+      <c r="D153" s="2">
         <v>0.3548</v>
       </c>
     </row>
@@ -2871,13 +2898,13 @@
       <c r="A154" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C154">
+      <c r="C154" s="2">
         <v>0.99219999999999997</v>
       </c>
-      <c r="D154">
+      <c r="D154" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -2885,13 +2912,13 @@
       <c r="A155" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C155">
+      <c r="C155" s="2">
         <v>0.79530000000000001</v>
       </c>
-      <c r="D155">
+      <c r="D155" s="2">
         <v>2E-3</v>
       </c>
     </row>
@@ -2899,13 +2926,13 @@
       <c r="A156" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C156">
+      <c r="C156" s="2">
         <v>0.88</v>
       </c>
-      <c r="D156">
+      <c r="D156" s="2">
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
@@ -2913,10 +2940,10 @@
       <c r="A157" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C157">
+      <c r="C157" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2924,13 +2951,13 @@
       <c r="A158" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C158">
+      <c r="C158" s="2">
         <v>0.87139999999999995</v>
       </c>
-      <c r="D158">
+      <c r="D158" s="2">
         <v>6.3E-2</v>
       </c>
     </row>
@@ -2938,10 +2965,10 @@
       <c r="A159" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C159">
+      <c r="C159" s="2">
         <v>0.63790000000000002</v>
       </c>
     </row>
@@ -2949,10 +2976,10 @@
       <c r="A160" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C160">
+      <c r="C160" s="2">
         <v>0.99</v>
       </c>
     </row>
@@ -2960,13 +2987,13 @@
       <c r="A161" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C161">
+      <c r="C161" s="2">
         <v>0.82550000000000001</v>
       </c>
-      <c r="D161">
+      <c r="D161" s="2">
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
@@ -2974,13 +3001,13 @@
       <c r="A162" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C162">
+      <c r="C162" s="2">
         <v>0.34279999999999999</v>
       </c>
-      <c r="D162">
+      <c r="D162" s="2">
         <v>0.1578</v>
       </c>
     </row>
@@ -2988,13 +3015,13 @@
       <c r="A163" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C163">
+      <c r="C163" s="2">
         <v>0.47099999999999997</v>
       </c>
-      <c r="D163">
+      <c r="D163" s="2">
         <v>0.34710000000000002</v>
       </c>
     </row>
@@ -3002,10 +3029,10 @@
       <c r="A164" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C164">
+      <c r="C164" s="2">
         <v>0.81869999999999998</v>
       </c>
     </row>
@@ -3013,13 +3040,13 @@
       <c r="A165" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="2">
         <v>0.53249999999999997</v>
       </c>
-      <c r="D165">
+      <c r="D165" s="2">
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
@@ -3027,12 +3054,12 @@
       <c r="A166" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B166">
+      <c r="B166" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D167">
+      <c r="D167" s="2">
         <v>0.45</v>
       </c>
     </row>
@@ -3054,10 +3081,10 @@
       <c r="A169" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="2">
         <v>0.92</v>
       </c>
     </row>
@@ -3065,13 +3092,13 @@
       <c r="A170" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="2">
         <v>0.83609999999999995</v>
       </c>
-      <c r="D170">
+      <c r="D170" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
@@ -3079,13 +3106,13 @@
       <c r="A171" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C171">
+      <c r="C171" s="2">
         <v>0.91879999999999995</v>
       </c>
-      <c r="D171">
+      <c r="D171" s="2">
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
@@ -3093,10 +3120,10 @@
       <c r="A172" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="2">
         <v>0.96</v>
       </c>
     </row>
@@ -3104,13 +3131,13 @@
       <c r="A173" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B173" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="2">
         <v>0.5927</v>
       </c>
-      <c r="D173">
+      <c r="D173" s="2">
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
@@ -3118,13 +3145,13 @@
       <c r="A174" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C174">
+      <c r="C174" s="2">
         <v>0.72</v>
       </c>
-      <c r="D174">
+      <c r="D174" s="2">
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
@@ -3132,10 +3159,10 @@
       <c r="A175" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C175">
+      <c r="C175" s="2">
         <v>0.64</v>
       </c>
     </row>
@@ -3143,13 +3170,13 @@
       <c r="A176" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B176" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C176">
+      <c r="C176" s="2">
         <v>0.57340000000000002</v>
       </c>
-      <c r="D176">
+      <c r="D176" s="2">
         <v>0.1973</v>
       </c>
     </row>
@@ -3157,13 +3184,13 @@
       <c r="A177" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="2">
         <v>0.63800000000000001</v>
       </c>
-      <c r="D177">
+      <c r="D177" s="2">
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
@@ -3171,13 +3198,13 @@
       <c r="A178" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="2">
         <v>0.59150000000000003</v>
       </c>
-      <c r="D178">
+      <c r="D178" s="2">
         <v>2.8999999999999998E-3</v>
       </c>
     </row>
@@ -3185,10 +3212,10 @@
       <c r="A179" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B179" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3196,13 +3223,13 @@
       <c r="A180" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="2">
         <v>0.64770000000000005</v>
       </c>
-      <c r="D180">
+      <c r="D180" s="2">
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
@@ -3210,13 +3237,13 @@
       <c r="A181" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="2">
         <v>0.98</v>
       </c>
-      <c r="D181">
+      <c r="D181" s="2">
         <v>1E-4</v>
       </c>
     </row>
@@ -3224,10 +3251,10 @@
       <c r="A182" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B182" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C182">
+      <c r="C182" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3235,13 +3262,13 @@
       <c r="A183" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B183" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D183">
+      <c r="D183" s="2">
         <v>0.4632</v>
       </c>
     </row>
@@ -3249,10 +3276,10 @@
       <c r="A184" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="2">
         <v>0.78</v>
       </c>
     </row>
@@ -3260,13 +3287,13 @@
       <c r="A185" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="2">
         <v>0.51819999999999999</v>
       </c>
-      <c r="D185">
+      <c r="D185" s="2">
         <v>0.21609999999999999</v>
       </c>
     </row>
@@ -3274,10 +3301,10 @@
       <c r="A186" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B186" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C186">
+      <c r="C186" s="2">
         <v>0.92949999999999999</v>
       </c>
     </row>
@@ -3285,10 +3312,10 @@
       <c r="A187" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C187">
+      <c r="C187" s="2">
         <v>0.51</v>
       </c>
     </row>
@@ -3296,7 +3323,7 @@
       <c r="A188" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3319,10 +3346,10 @@
       <c r="A191" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C191">
+      <c r="C191" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3330,10 +3357,10 @@
       <c r="A192" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C192">
+      <c r="C192" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3341,10 +3368,10 @@
       <c r="A193" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C193">
+      <c r="C193" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3352,10 +3379,10 @@
       <c r="A194" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C194">
+      <c r="C194" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3363,10 +3390,10 @@
       <c r="A195" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C195">
+      <c r="C195" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3374,10 +3401,10 @@
       <c r="A196" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3385,10 +3412,10 @@
       <c r="A197" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B197" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C197">
+      <c r="C197" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3396,10 +3423,10 @@
       <c r="A198" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C198">
+      <c r="C198" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3407,10 +3434,10 @@
       <c r="A199" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C199">
+      <c r="C199" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3418,10 +3445,10 @@
       <c r="A200" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3434,10 +3461,10 @@
       <c r="A202" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C202">
+      <c r="C202" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3445,7 +3472,7 @@
       <c r="A203" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B203" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3458,10 +3485,10 @@
       <c r="A205" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C205">
+      <c r="C205" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3469,10 +3496,10 @@
       <c r="A206" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B206" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C206">
+      <c r="C206" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3480,10 +3507,10 @@
       <c r="A207" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B207" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C207">
+      <c r="C207" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3491,10 +3518,10 @@
       <c r="A208" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B208" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C208">
+      <c r="C208" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3502,10 +3529,10 @@
       <c r="A209" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B209" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C209">
+      <c r="C209" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3533,10 +3560,10 @@
       <c r="A213" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B213" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C213">
+      <c r="C213" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3544,10 +3571,10 @@
       <c r="A214" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C214">
+      <c r="C214" s="2">
         <v>0.9365</v>
       </c>
     </row>
@@ -3555,10 +3582,10 @@
       <c r="A215" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B215" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C215">
+      <c r="C215" s="2">
         <v>0.94920000000000004</v>
       </c>
     </row>
@@ -3566,10 +3593,10 @@
       <c r="A216" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B216" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C216">
+      <c r="C216" s="2">
         <v>0.99739999999999995</v>
       </c>
     </row>
@@ -3577,10 +3604,10 @@
       <c r="A217" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B217" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C217">
+      <c r="C217" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3588,10 +3615,10 @@
       <c r="A218" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B218" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C218">
+      <c r="C218" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3599,10 +3626,10 @@
       <c r="A219" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B219" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C219">
+      <c r="C219" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3610,10 +3637,10 @@
       <c r="A220" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B220" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C220">
+      <c r="C220" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3621,10 +3648,10 @@
       <c r="A221" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B221" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C221">
+      <c r="C221" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3632,10 +3659,10 @@
       <c r="A222" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B222" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C222">
+      <c r="C222" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3643,13 +3670,13 @@
       <c r="A223" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B223" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C223">
+      <c r="C223" s="2">
         <v>0.32500000000000001</v>
       </c>
-      <c r="D223">
+      <c r="D223" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -3657,10 +3684,10 @@
       <c r="A224" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B224" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C224">
+      <c r="C224" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3668,10 +3695,10 @@
       <c r="A225" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B225" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C225">
+      <c r="C225" s="2">
         <v>0.99</v>
       </c>
     </row>
@@ -3679,13 +3706,13 @@
       <c r="A226" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B226" t="s">
+      <c r="B226" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C226">
+      <c r="C226" s="2">
         <v>0.99839999999999995</v>
       </c>
-      <c r="D226">
+      <c r="D226" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3693,10 +3720,10 @@
       <c r="A227" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B227" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C227">
+      <c r="C227" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3704,10 +3731,10 @@
       <c r="A228" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B228" t="s">
+      <c r="B228" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C228">
+      <c r="C228" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3715,10 +3742,10 @@
       <c r="A229" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B229" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C229">
+      <c r="C229" s="2">
         <v>0.85</v>
       </c>
     </row>
@@ -3726,13 +3753,13 @@
       <c r="A230" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B230" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C230">
+      <c r="C230" s="2">
         <v>0.99780000000000002</v>
       </c>
-      <c r="D230">
+      <c r="D230" s="2">
         <v>1E-3</v>
       </c>
     </row>
@@ -3740,10 +3767,10 @@
       <c r="A231" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B231" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C231">
+      <c r="C231" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3751,14 +3778,362 @@
       <c r="A232" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B232" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C232">
+      <c r="C232" s="2">
         <v>0.83340000000000003</v>
       </c>
-      <c r="D232">
+      <c r="D232" s="2">
         <v>5.2600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B234" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C234" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D234" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A235" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C235" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C236" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C237" s="2">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A238" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C238" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A239" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C239" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A240" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C240" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A241" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C241" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A242" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B242" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C242" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A243" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B243" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C243" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A244" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B244" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C244" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A245" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B245" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C245" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A246" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B246" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C246" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A247" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B247" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C247" s="2">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A248" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B248" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C248" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A249" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B249" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C249" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A250" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B250" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C250" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A251" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B251" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C251" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A252" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B252" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C252" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A253" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B253" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C253" s="2">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="D253" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A254" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B254" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C254" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A255" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B255" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C255" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A256" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B256" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C256" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A257" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B257" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C257" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A258" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B258" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C258" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A259" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B259" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C259" s="2">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A260" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B260" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C260" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A261" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B261" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C261" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A262" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B262" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C262" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A263" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B263" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C263" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A264" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B264" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C264" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started working on 40 words
</commit_message>
<xml_diff>
--- a/translate/record of results.xlsx
+++ b/translate/record of results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\COS301\Hands-Up\translate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D91595-5CC4-4DD3-AE22-30D48E55B7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7A779D-49D9-4168-88DF-C2AD7A390AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="0" windowWidth="8688" windowHeight="12336" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
+    <workbookView xWindow="12876" yWindow="1440" windowWidth="8688" windowHeight="8880" xr2:uid="{160F58D6-6A9C-4BF1-8413-2E72D986BFF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="60">
   <si>
     <t>sign</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t xml:space="preserve">future </t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -313,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,148 +342,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="44">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -492,12 +359,18 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -524,6 +397,25 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -548,6 +440,15 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -556,12 +457,18 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -588,6 +495,25 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -612,6 +538,15 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -620,12 +555,18 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -652,6 +593,25 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -676,6 +636,15 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -684,12 +653,18 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -716,6 +691,25 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -739,6 +733,12 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -753,48 +753,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DD2ABC0D-50C1-49C4-8D3A-5CA063F1F218}" name="Table5" displayName="Table5" ref="A2:D12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DD2ABC0D-50C1-49C4-8D3A-5CA063F1F218}" name="Table5" displayName="Table5" ref="A2:D12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F400AB7F-4E8B-4125-9E25-5ED9FB65B14F}" name="Column1" headerRowDxfId="42" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{3F22CA1A-5693-4313-92A4-EE54C2FDC4CF}" name="Test 1" headerRowDxfId="41" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{788734D9-F3D0-4322-87BC-6A1CAF964241}" name="Column2" headerRowDxfId="40" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{4FC0C234-7164-459C-8403-515A895D477E}" name="Column3" headerRowDxfId="39" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{F400AB7F-4E8B-4125-9E25-5ED9FB65B14F}" name="Column1" headerRowDxfId="40" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{3F22CA1A-5693-4313-92A4-EE54C2FDC4CF}" name="Test 1" headerRowDxfId="38" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{788734D9-F3D0-4322-87BC-6A1CAF964241}" name="Column2" headerRowDxfId="36" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{4FC0C234-7164-459C-8403-515A895D477E}" name="Column3" headerRowDxfId="34" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E569A974-8B60-4556-8570-6A44C4FBD727}" name="Table57" displayName="Table57" ref="A16:D26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E569A974-8B60-4556-8570-6A44C4FBD727}" name="Table57" displayName="Table57" ref="A16:D26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8766D2EA-8EEA-45A1-8B07-7FA7D5ACC38E}" name="Column1" headerRowDxfId="37" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{A099EBA9-F36A-46FA-BDB1-F7CAF089E494}" name="Test 1" headerRowDxfId="36" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{92A9AE78-3CB8-4AAA-8266-990E00ABEE53}" name="Column2" headerRowDxfId="35" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{8468543C-F567-482E-BE69-7F793167F224}" name="Column3" headerRowDxfId="34" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{8766D2EA-8EEA-45A1-8B07-7FA7D5ACC38E}" name="Column1" headerRowDxfId="29" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{A099EBA9-F36A-46FA-BDB1-F7CAF089E494}" name="Test 1" headerRowDxfId="27" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{92A9AE78-3CB8-4AAA-8266-990E00ABEE53}" name="Column2" headerRowDxfId="25" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{8468543C-F567-482E-BE69-7F793167F224}" name="Column3" headerRowDxfId="23" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1C6A1CC9-8976-4B5C-B94C-E8A89F240FFB}" name="Table578" displayName="Table578" ref="A29:D39" headerRowCount="0" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1C6A1CC9-8976-4B5C-B94C-E8A89F240FFB}" name="Table578" displayName="Table578" ref="A29:D39" headerRowCount="0" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E504D3A5-FC9A-45F6-8C0E-D7A50AF19A75}" name="Column1" headerRowDxfId="32" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{6EAF6B0D-E32F-4ABE-93B4-E394AE2A7E61}" name="Test 1" headerRowDxfId="31" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{8BDDF0B1-E9A5-48D4-B164-ADE5E3372319}" name="Column2" headerRowDxfId="30" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{CD0DB33E-E98F-4D80-969C-C6CB71E17312}" name="Column3" headerRowDxfId="29" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{E504D3A5-FC9A-45F6-8C0E-D7A50AF19A75}" name="Column1" headerRowDxfId="18" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{6EAF6B0D-E32F-4ABE-93B4-E394AE2A7E61}" name="Test 1" headerRowDxfId="16" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{8BDDF0B1-E9A5-48D4-B164-ADE5E3372319}" name="Column2" headerRowDxfId="14" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{CD0DB33E-E98F-4D80-969C-C6CB71E17312}" name="Column3" headerRowDxfId="12" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{2B773CE3-EB5B-45E6-9DCA-44D0A01FB542}" name="Table5789" displayName="Table5789" ref="A42:D52" headerRowCount="0" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{2B773CE3-EB5B-45E6-9DCA-44D0A01FB542}" name="Table5789" displayName="Table5789" ref="A42:D52" headerRowCount="0" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DC2E491C-2CD4-4E89-AC71-91DE1A7E1452}" name="Column1" headerRowDxfId="27" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{BE664661-355B-4988-923D-8558A307F1DC}" name="Test 1" headerRowDxfId="26" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{E149DA85-C608-4816-AFAC-5502546D39B6}" name="Column2" headerRowDxfId="25" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{0BD5DA97-7603-4D27-9BC6-3BFD8A154644}" name="Column3" headerRowDxfId="24" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{DC2E491C-2CD4-4E89-AC71-91DE1A7E1452}" name="Column1" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{BE664661-355B-4988-923D-8558A307F1DC}" name="Test 1" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{E149DA85-C608-4816-AFAC-5502546D39B6}" name="Column2" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{0BD5DA97-7603-4D27-9BC6-3BFD8A154644}" name="Column3" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1119,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBF13E0-78B5-4465-B2C7-E04C9FCCA561}">
   <dimension ref="A1:E264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A235" sqref="A235:A264"/>
+    <sheetView tabSelected="1" topLeftCell="A239" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C252" sqref="C252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3884,7 +3884,7 @@
       <c r="A242" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B242" s="9" t="s">
+      <c r="B242" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C242" s="2">
@@ -3895,7 +3895,7 @@
       <c r="A243" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B243" s="9" t="s">
+      <c r="B243" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C243" s="2">
@@ -3906,7 +3906,7 @@
       <c r="A244" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B244" s="9" t="s">
+      <c r="B244" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C244" s="2">
@@ -3917,7 +3917,7 @@
       <c r="A245" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B245" s="9" t="s">
+      <c r="B245" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C245" s="2">
@@ -3928,7 +3928,7 @@
       <c r="A246" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B246" s="9" t="s">
+      <c r="B246" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C246" s="2">
@@ -3939,7 +3939,7 @@
       <c r="A247" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B247" s="9" t="s">
+      <c r="B247" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C247" s="2">
@@ -3950,7 +3950,7 @@
       <c r="A248" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B248" s="9" t="s">
+      <c r="B248" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C248" s="2">
@@ -3961,7 +3961,7 @@
       <c r="A249" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B249" s="9" t="s">
+      <c r="B249" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C249" s="2">
@@ -3972,7 +3972,7 @@
       <c r="A250" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B250" s="9" t="s">
+      <c r="B250" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C250" s="2">
@@ -3983,7 +3983,7 @@
       <c r="A251" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B251" s="9" t="s">
+      <c r="B251" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C251" s="2">
@@ -3994,18 +3994,18 @@
       <c r="A252" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B252" s="9" t="s">
+      <c r="B252" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C252" s="2">
-        <v>1</v>
+      <c r="C252" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B253" s="9" t="s">
+      <c r="B253" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C253" s="2">
@@ -4019,7 +4019,7 @@
       <c r="A254" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B254" s="9" t="s">
+      <c r="B254" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C254" s="2">
@@ -4030,7 +4030,7 @@
       <c r="A255" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B255" s="9" t="s">
+      <c r="B255" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C255" s="2">
@@ -4041,7 +4041,7 @@
       <c r="A256" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B256" s="9" t="s">
+      <c r="B256" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C256" s="2">
@@ -4052,7 +4052,7 @@
       <c r="A257" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B257" s="9" t="s">
+      <c r="B257" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C257" s="2">
@@ -4063,7 +4063,7 @@
       <c r="A258" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B258" s="9" t="s">
+      <c r="B258" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C258" s="2">
@@ -4074,7 +4074,7 @@
       <c r="A259" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B259" s="9" t="s">
+      <c r="B259" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C259" s="2">
@@ -4085,7 +4085,7 @@
       <c r="A260" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B260" s="9" t="s">
+      <c r="B260" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C260" s="2">
@@ -4096,7 +4096,7 @@
       <c r="A261" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B261" s="9" t="s">
+      <c r="B261" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C261" s="2">
@@ -4107,7 +4107,7 @@
       <c r="A262" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B262" s="9" t="s">
+      <c r="B262" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C262" s="2">
@@ -4118,7 +4118,7 @@
       <c r="A263" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B263" s="9" t="s">
+      <c r="B263" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C263" s="2">
@@ -4129,7 +4129,7 @@
       <c r="A264" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B264" s="9" t="s">
+      <c r="B264" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C264" s="2">

</xml_diff>